<commit_message>
feat: Generate more realistic sample compliance data with dynamic backup dates and retention periods.
</commit_message>
<xml_diff>
--- a/sample_compliance.xlsx
+++ b/sample_compliance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>backup_type</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>retention_days</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -473,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,6 +490,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F2" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +508,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -512,6 +520,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F3" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -527,7 +538,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -539,6 +550,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +568,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -566,6 +580,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F5" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -581,7 +598,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -593,6 +610,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F6" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -608,7 +628,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -620,6 +640,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F7" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -635,7 +658,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -647,6 +670,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F8" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -662,7 +688,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -674,6 +700,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F9" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -689,7 +718,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -701,6 +730,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F10" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="11">
@@ -716,7 +748,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -728,6 +760,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F11" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -743,7 +778,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -755,6 +790,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F12" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="13">
@@ -770,7 +808,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -782,6 +820,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="14">
@@ -797,7 +838,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -809,6 +850,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F14" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="15">
@@ -824,7 +868,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -836,6 +880,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F15" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -851,7 +898,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -863,6 +910,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F16" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="17">
@@ -878,7 +928,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -890,6 +940,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F17" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="18">
@@ -905,7 +958,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-15</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -917,6 +970,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F18" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="19">
@@ -932,7 +988,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -944,6 +1000,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F19" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="20">
@@ -959,7 +1018,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -971,6 +1030,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F20" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="21">
@@ -986,7 +1048,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -998,6 +1060,9 @@
         <is>
           <t>full</t>
         </is>
+      </c>
+      <c r="F21" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>